<commit_message>
menghapus komentar pada code rules di line 63 - 76
</commit_message>
<xml_diff>
--- a/peringkat.xlsx
+++ b/peringkat.xlsx
@@ -441,17 +441,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nama</t>
+          <t>id Pelanggan</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Kualitas</t>
+          <t>Pelayanan</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Harga</t>
+          <t>harga</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">

</xml_diff>